<commit_message>
login functionality validation with pom
</commit_message>
<xml_diff>
--- a/src/main/java/com/streams/testdata/logindata.xlsx
+++ b/src/main/java/com/streams/testdata/logindata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -22,13 +22,37 @@
     <t>password</t>
   </si>
   <si>
+    <t>inputdata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected </t>
+  </si>
+  <si>
     <t>sameerone@accountvalidation</t>
   </si>
   <si>
     <t>abc@1234</t>
   </si>
   <si>
-    <t>sameertwo@accountvalidation</t>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>https://streams.us/sloader/home.jsp</t>
+  </si>
+  <si>
+    <t>abc@12345</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>https://accounts.unifiedcloudit.com/auth/SSOLogin</t>
+  </si>
+  <si>
+    <t>sameeronee@accountvalidation</t>
+  </si>
+  <si>
+    <t>https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10</t>
   </si>
 </sst>
 </file>
@@ -37,9 +61,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -59,6 +83,97 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -74,110 +189,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -185,14 +217,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -217,19 +241,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +343,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,151 +409,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,11 +435,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -435,17 +465,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,15 +537,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -531,31 +555,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -564,109 +588,121 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -987,48 +1023,104 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="34.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="28.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="34.5714285714286" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1428571428571" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5714285714286" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="30" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="sameerone@accountvalidation"/>
+    <hyperlink ref="A2" r:id="rId1" display="sameerone@accountvalidation" tooltip="mailto:sameerone@accountvalidation"/>
     <hyperlink ref="B2" r:id="rId2" display="abc@1234"/>
-    <hyperlink ref="A3" r:id="rId3" display="sameertwo@accountvalidation"/>
-    <hyperlink ref="B3" r:id="rId2" display="abc@1234"/>
+    <hyperlink ref="A5" r:id="rId3" display="sameeronee@accountvalidation" tooltip="mailto:sameeronee@accountvalidation"/>
+    <hyperlink ref="B5" r:id="rId4" display="abc@12345"/>
+    <hyperlink ref="A3" r:id="rId1" display="sameerone@accountvalidation" tooltip="mailto:sameerone@accountvalidation"/>
+    <hyperlink ref="B3" r:id="rId4" display="abc@12345"/>
+    <hyperlink ref="A4" r:id="rId3" display="sameeronee@accountvalidation" tooltip="mailto:sameeronee@accountvalidation"/>
+    <hyperlink ref="B4" r:id="rId2" display="abc@1234"/>
+    <hyperlink ref="D5" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10"/>
+    <hyperlink ref="D3" r:id="rId6" display="https://accounts.unifiedcloudit.com/auth/SSOLogin" tooltip="https://accounts.unifiedcloudit.com/auth/SSOLogin"/>
+    <hyperlink ref="D4" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
changes done login testcase
</commit_message>
<xml_diff>
--- a/src/main/java/com/streams/testdata/logindata.xlsx
+++ b/src/main/java/com/streams/testdata/logindata.xlsx
@@ -52,7 +52,7 @@
     <t>sameeronee@accountvalidation</t>
   </si>
   <si>
-    <t>https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10</t>
+    <t>https://accounts.wspbx.com/auth/index.jsp?dashboardid</t>
   </si>
 </sst>
 </file>
@@ -60,9 +60,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -103,46 +103,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,14 +157,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -187,23 +173,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,13 +204,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -227,6 +213,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,19 +247,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,13 +373,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,85 +391,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,49 +421,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,21 +432,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -469,7 +454,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,7 +478,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,15 +515,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -532,20 +523,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -558,131 +558,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -695,14 +695,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1034,7 +1028,7 @@
     <col min="1" max="1" width="34.5714285714286" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.1428571428571" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5714285714286" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.1428571428571" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
@@ -1062,7 +1056,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1076,11 +1070,11 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="30" spans="1:4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1090,11 +1084,11 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1098,7 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1118,9 +1112,8 @@
     <hyperlink ref="B3" r:id="rId4" display="abc@12345"/>
     <hyperlink ref="A4" r:id="rId3" display="sameeronee@accountvalidation" tooltip="mailto:sameeronee@accountvalidation"/>
     <hyperlink ref="B4" r:id="rId2" display="abc@1234"/>
-    <hyperlink ref="D5" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10"/>
-    <hyperlink ref="D3" r:id="rId6" display="https://accounts.unifiedcloudit.com/auth/SSOLogin" tooltip="https://accounts.unifiedcloudit.com/auth/SSOLogin"/>
-    <hyperlink ref="D4" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid=302922967&amp;src=streams.us&amp;svid=10"/>
+    <hyperlink ref="D4" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid"/>
+    <hyperlink ref="D5" r:id="rId5" display="https://accounts.wspbx.com/auth/index.jsp?dashboardid"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>